<commit_message>
Calcul des BeatTime pour les WarpMarker relativement au début de l'AudioClip
</commit_message>
<xml_diff>
--- a/resources/Excel/sample.xlsx
+++ b/resources/Excel/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>BeatTime</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,6 +33,34 @@
   </si>
   <si>
     <t>Accélération</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Section</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Couplet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mini Refrain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refrain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pont sensuel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Couplet mineur</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -389,1319 +417,2362 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:10">
+      <c r="A2">
+        <v>16</v>
+      </c>
       <c r="B2">
-        <v>5.612108843537415</v>
+        <v>1.4676190476190476</v>
       </c>
       <c r="C2">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>69.81726070816629</v>
+        <v>68.67554309740714</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>33.1124716553288</v>
+        <v>4.962312925170068</v>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>68.97843934977523</v>
+        <v>69.33825986124486</v>
       </c>
       <c r="E3">
-        <v>-0.026213167449720576</v>
+        <v>0.1656791909594304</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>60.947256235827666</v>
+        <v>8.423605442176871</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>73.84512338917318</v>
+        <v>68.38136956563876</v>
       </c>
       <c r="E4">
-        <v>0.15208387623118602</v>
+        <v>-0.23922257390152524</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>64.19730158730158</v>
+        <v>11.933333333333334</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>71.76008964463887</v>
+        <v>67.44064535039317</v>
       </c>
       <c r="E5">
-        <v>-0.5212584361335786</v>
+        <v>-0.23518105381139875</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="B6">
-        <v>100.98655328798186</v>
+        <v>15.492018140589568</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>72.24129575657469</v>
+        <v>68.31053411170167</v>
       </c>
       <c r="E6">
-        <v>0.010936502543995889</v>
+        <v>0.2174721903271255</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="B7">
-        <v>110.95315192743764</v>
+        <v>22.51875283446712</v>
       </c>
       <c r="C7">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>71.81508836092104</v>
+        <v>69.25432512366838</v>
       </c>
       <c r="E7">
-        <v>-0.035517282971137355</v>
+        <v>0.11797387649583868</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>164</v>
+        <v>44</v>
       </c>
       <c r="B8">
-        <v>144.37231292517006</v>
+        <v>25.984240362811793</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>70.64467942240093</v>
+        <v>68.34516114451023</v>
       </c>
       <c r="E8">
-        <v>-0.029260223463002787</v>
+        <v>-0.22729099478953785</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>184</v>
+        <v>48</v>
       </c>
       <c r="B9">
-        <v>161.35873015873017</v>
+        <v>29.495827664399094</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>70.91338503542666</v>
+        <v>67.45740890636655</v>
       </c>
       <c r="E9">
-        <v>0.013435280651286519</v>
+        <v>-0.22193805953591905</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>192</v>
+        <v>52</v>
       </c>
       <c r="B10">
-        <v>168.12755102040816</v>
+        <v>33.05362811791383</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D10">
-        <v>73.94779498071648</v>
+        <v>68.25700853212606</v>
       </c>
       <c r="E10">
-        <v>0.37930124316122793</v>
+        <v>0.1998999064398781</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>196</v>
+        <v>64</v>
       </c>
       <c r="B11">
-        <v>171.37308390022676</v>
+        <v>43.60199546485261</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>68.8403676169291</v>
+        <v>69.4706994328922</v>
       </c>
       <c r="E11">
-        <v>-1.276856840946845</v>
+        <v>0.10114090839717822</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>200</v>
+        <v>68</v>
       </c>
       <c r="B12">
-        <v>174.859410430839</v>
+        <v>47.05668934240363</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>71.27320722698487</v>
+        <v>68.58698117486963</v>
       </c>
       <c r="E12">
-        <v>0.6082099025139414</v>
+        <v>-0.22092956450564216</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>208</v>
+        <v>72</v>
       </c>
       <c r="B13">
-        <v>181.5940589569161</v>
+        <v>50.555895691609976</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>70.511112295475</v>
+        <v>67.95592880807457</v>
       </c>
       <c r="E13">
-        <v>-0.09526186643873302</v>
+        <v>-0.15776309169876512</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>212</v>
+        <v>84</v>
       </c>
       <c r="B14">
-        <v>184.99777777777777</v>
+        <v>61.150997732426305</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14">
-        <v>71.31402697858685</v>
+        <v>68.31957345451508</v>
       </c>
       <c r="E14">
-        <v>0.20072867077796275</v>
+        <v>0.030303720536708784</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>216</v>
+        <v>88</v>
       </c>
       <c r="B15">
-        <v>188.3631746031746</v>
+        <v>64.66390022675736</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15">
-        <v>72.20039292730812</v>
+        <v>67.64452113891285</v>
       </c>
       <c r="E15">
-        <v>0.22159148718031574</v>
+        <v>-0.16876307890055742</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>220</v>
+        <v>92</v>
       </c>
       <c r="B16">
-        <v>191.68725623582768</v>
+        <v>68.21185941043083</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16">
-        <v>70.66175292421082</v>
+        <v>68.72950420468183</v>
       </c>
       <c r="E16">
-        <v>-0.38466000077432483</v>
+        <v>0.2712457664422452</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>224</v>
+        <v>96</v>
       </c>
       <c r="B17">
-        <v>195.0837188208617</v>
+        <v>71.70380952380953</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17">
-        <v>69.34053119144644</v>
+        <v>69.21718658034146</v>
       </c>
       <c r="E17">
-        <v>-0.33030543319109285</v>
+        <v>0.12192059391490773</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>228</v>
+        <v>100</v>
       </c>
       <c r="B18">
-        <v>198.5448979591837</v>
+        <v>75.17115646258503</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18">
-        <v>70.54683125816521</v>
+        <v>68.6782168580883</v>
       </c>
       <c r="E18">
-        <v>0.301575016679692</v>
+        <v>-0.13474243056328916</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>232</v>
+        <v>104</v>
       </c>
       <c r="B19">
-        <v>201.9468934240363</v>
+        <v>78.66571428571429</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>71.30874178878217</v>
+        <v>69.19139422228331</v>
       </c>
       <c r="E19">
-        <v>0.19047763265423967</v>
+        <v>0.12829434104875048</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>236</v>
+        <v>112</v>
       </c>
       <c r="B20">
-        <v>205.3125396825397</v>
+        <v>85.6029931972789</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20">
-        <v>71.9862883260335</v>
+        <v>69.55241731450378</v>
       </c>
       <c r="E20">
-        <v>0.16938663431283274</v>
+        <v>0.045127886527559724</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>240</v>
+        <v>116</v>
       </c>
       <c r="B21">
-        <v>208.64650793650793</v>
+        <v>89.05362811791383</v>
       </c>
       <c r="C21">
         <v>8</v>
       </c>
       <c r="D21">
-        <v>72.65762565259023</v>
+        <v>69.78101131040482</v>
       </c>
       <c r="E21">
-        <v>0.16783433163918104</v>
+        <v>0.05714849897525909</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>248</v>
+        <v>124</v>
       </c>
       <c r="B22">
-        <v>215.25283446712018</v>
+        <v>95.93229024943311</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <v>75.83128542053265</v>
+        <v>68.81373674064494</v>
       </c>
       <c r="E22">
-        <v>0.3967074709928031</v>
+        <v>-0.12090932121998499</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>252</v>
+        <v>132</v>
       </c>
       <c r="B23">
-        <v>218.41775510204081</v>
+        <v>102.90764172335601</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23">
-        <v>74.78748736936575</v>
+        <v>69.04334779347016</v>
       </c>
       <c r="E23">
-        <v>-0.2609495127917256</v>
+        <v>0.028701381603152498</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>256</v>
+        <v>136</v>
       </c>
       <c r="B24">
-        <v>221.62684807256235</v>
+        <v>106.38371882086167</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>74.33628318584073</v>
+        <v>68.65393783912639</v>
       </c>
       <c r="E24">
-        <v>-0.11280104588125539</v>
+        <v>-0.09735248858594403</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>260</v>
+        <v>144</v>
       </c>
       <c r="B25">
-        <v>224.85541950113378</v>
+        <v>113.37530612244898</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D25">
-        <v>74.70883038046131</v>
+        <v>67.7391173562287</v>
       </c>
       <c r="E25">
-        <v>0.09313679865514501</v>
+        <v>-0.1143525603622102</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>264</v>
+        <v>152</v>
       </c>
       <c r="B26">
-        <v>228.0678911564626</v>
+        <v>120.46131519274377</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D26">
-        <v>75.32640374069892</v>
+        <v>68.58120367010518</v>
       </c>
       <c r="E26">
-        <v>0.15439334005940353</v>
+        <v>0.10526078923455984</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>272</v>
+        <v>156</v>
       </c>
       <c r="B27">
-        <v>234.44015873015874</v>
+        <v>123.96081632653062</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27">
-        <v>74.3315846027437</v>
+        <v>68.81575012028463</v>
       </c>
       <c r="E27">
-        <v>-0.12435239224440231</v>
+        <v>0.05863661254486274</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28">
-        <v>276</v>
+        <v>160</v>
       </c>
       <c r="B28">
-        <v>237.6689342403628</v>
+        <v>127.44839002267574</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28">
-        <v>75.64052170805748</v>
+        <v>69.36552564833553</v>
       </c>
       <c r="E28">
-        <v>0.3272342763284435</v>
+        <v>0.13744388201272528</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29">
-        <v>280</v>
+        <v>164</v>
       </c>
       <c r="B29">
-        <v>240.84183673469389</v>
+        <v>130.90832199546486</v>
       </c>
       <c r="C29">
         <v>8</v>
       </c>
       <c r="D29">
-        <v>74.24763240968105</v>
+        <v>68.76187691857933</v>
       </c>
       <c r="E29">
-        <v>-0.34822232459410785</v>
+        <v>-0.15091218243905047</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30">
-        <v>288</v>
+        <v>172</v>
       </c>
       <c r="B30">
-        <v>247.30668934240362</v>
+        <v>137.8889342403628</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
       <c r="D30">
-        <v>73.67292673079851</v>
+        <v>68.96102372978524</v>
       </c>
       <c r="E30">
-        <v>-0.07183820986031719</v>
+        <v>0.02489335140073834</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31">
-        <v>292</v>
+        <v>176</v>
       </c>
       <c r="B31">
-        <v>250.56433106575963</v>
+        <v>141.36916099773242</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D31">
-        <v>75.0388168482844</v>
+        <v>69.37029936587528</v>
       </c>
       <c r="E31">
-        <v>0.34147252937147243</v>
+        <v>0.10231890902251095</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32">
-        <v>296</v>
+        <v>184</v>
       </c>
       <c r="B32">
-        <v>253.76267573696146</v>
+        <v>148.28854875283446</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32">
-        <v>74.44818029627339</v>
+        <v>69.57756478523258</v>
       </c>
       <c r="E32">
-        <v>-0.14765913800275143</v>
+        <v>0.025908177419662337</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32">
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33">
-        <v>300</v>
+        <v>188</v>
       </c>
       <c r="B33">
-        <v>256.98639455782313</v>
+        <v>151.7379365079365</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33">
-        <v>75.56006111055636</v>
+        <v>67.77403532138854</v>
       </c>
       <c r="E33">
-        <v>0.2779702035707423</v>
+        <v>-0.45088236596101083</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
-        <v>304</v>
+        <v>192</v>
       </c>
       <c r="B34">
-        <v>260.16267573696143</v>
+        <v>155.2791156462585</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34">
-        <v>73.46020905342942</v>
+        <v>68.64124830569509</v>
       </c>
       <c r="E34">
-        <v>-0.5249630142817345</v>
+        <v>0.21680324607663692</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35">
-        <v>308</v>
+        <v>196</v>
       </c>
       <c r="B35">
-        <v>263.4297505668934</v>
+        <v>158.77555555555554</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>74.00260099844782</v>
+        <v>69.4315065797242</v>
       </c>
       <c r="E35">
-        <v>0.13559798625459862</v>
+        <v>0.19756456850727844</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36">
-        <v>312</v>
+        <v>204</v>
       </c>
       <c r="B36">
-        <v>266.6728798185941</v>
+        <v>165.68884353741495</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
       <c r="D36">
-        <v>71.81825584235739</v>
+        <v>71.8557995858648</v>
       </c>
       <c r="E36">
-        <v>-0.5460862890226075</v>
+        <v>0.3030366257675752</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37">
-        <v>316</v>
+        <v>208</v>
       </c>
       <c r="B37">
-        <v>270.0146485260771</v>
+        <v>169.02886621315193</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
       <c r="D37">
-        <v>71.23099598215225</v>
+        <v>70.92027499698492</v>
       </c>
       <c r="E37">
-        <v>-0.14681496505128422</v>
+        <v>-0.23388114721997155</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
-        <v>320</v>
+        <v>212</v>
       </c>
       <c r="B38">
-        <v>273.38396825396825</v>
+        <v>172.41294784580498</v>
       </c>
       <c r="C38">
         <v>4</v>
       </c>
       <c r="D38">
-        <v>70.90507134722309</v>
+        <v>69.48073261996971</v>
       </c>
       <c r="E38">
-        <v>-0.08148115873229145</v>
+        <v>-0.3598855942538002</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
-        <v>324</v>
+        <v>216</v>
       </c>
       <c r="B39">
-        <v>276.7687755102041</v>
+        <v>175.86714285714285</v>
       </c>
       <c r="C39">
         <v>4</v>
       </c>
       <c r="D39">
-        <v>71.28808901581513</v>
+        <v>70.50970307847052</v>
       </c>
       <c r="E39">
-        <v>0.09575441714801158</v>
+        <v>0.25724261462520204</v>
+      </c>
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
-        <v>328</v>
+        <v>220</v>
       </c>
       <c r="B40">
-        <v>280.1353968253968</v>
+        <v>179.27092970521542</v>
       </c>
       <c r="C40">
         <v>4</v>
       </c>
       <c r="D40">
-        <v>71.95398860592476</v>
+        <v>69.08300534570891</v>
       </c>
       <c r="E40">
-        <v>0.16647489752740796</v>
+        <v>-0.3566744331904026</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40">
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41">
-        <v>332</v>
+        <v>224</v>
       </c>
       <c r="B41">
-        <v>283.47086167800455</v>
+        <v>182.74501133786848</v>
       </c>
       <c r="C41">
         <v>4</v>
       </c>
       <c r="D41">
-        <v>71.17399432437207</v>
+        <v>68.58431451325453</v>
       </c>
       <c r="E41">
-        <v>-0.19499857038817225</v>
+        <v>-0.12467270811359654</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42">
-        <v>336</v>
+        <v>228</v>
       </c>
       <c r="B42">
-        <v>286.8428798185941</v>
+        <v>186.2443537414966</v>
       </c>
       <c r="C42">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>71.35561510845903</v>
+        <v>68.34383717326173</v>
       </c>
       <c r="E42">
-        <v>0.04540519602173987</v>
+        <v>-0.060119334998198326</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43">
-        <v>344</v>
+        <v>232</v>
       </c>
       <c r="B43">
-        <v>293.56975056689345</v>
+        <v>189.7560090702948</v>
       </c>
       <c r="C43">
         <v>4</v>
       </c>
       <c r="D43">
-        <v>71.13476893297926</v>
+        <v>68.07481540559361</v>
       </c>
       <c r="E43">
-        <v>-0.027605771934972267</v>
+        <v>-0.06725544191703037</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44">
-        <v>348</v>
+        <v>236</v>
       </c>
       <c r="B44">
-        <v>296.9436281179138</v>
+        <v>193.28154195011336</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D44">
-        <v>72.11504066010036</v>
+        <v>68.46762925011633</v>
       </c>
       <c r="E44">
-        <v>0.24506793178027664</v>
+        <v>0.09820346113068013</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44">
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45">
-        <v>356</v>
+        <v>240</v>
       </c>
       <c r="B45">
-        <v>303.5996598639456</v>
+        <v>196.78684807256235</v>
       </c>
       <c r="C45">
         <v>4</v>
       </c>
       <c r="D45">
-        <v>71.73745069067017</v>
+        <v>69.32281876117554</v>
       </c>
       <c r="E45">
-        <v>-0.04719874617877373</v>
+        <v>0.21379737776480212</v>
+      </c>
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45">
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46">
-        <v>360</v>
+        <v>244</v>
       </c>
       <c r="B46">
-        <v>306.94519274376415</v>
+        <v>200.24891156462584</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46">
-        <v>72.79029462738235</v>
+        <v>69.08165263364022</v>
       </c>
       <c r="E46">
-        <v>0.2632109841780448</v>
+        <v>-0.06029153188383063</v>
+      </c>
+      <c r="F46" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
-        <v>364</v>
+        <v>248</v>
       </c>
       <c r="B47">
-        <v>310.24233560090704</v>
+        <v>203.72306122448978</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D47">
-        <v>73.2700135685207</v>
+        <v>69.24616934692426</v>
       </c>
       <c r="E47">
-        <v>0.11992973528458606</v>
+        <v>0.04112917832101104</v>
+      </c>
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48">
-        <v>368</v>
+        <v>260</v>
       </c>
       <c r="B48">
-        <v>313.5178911564626</v>
+        <v>214.12074829931973</v>
       </c>
       <c r="C48">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D48">
-        <v>72.29137851544513</v>
+        <v>68.81530269240513</v>
       </c>
       <c r="E48">
-        <v>-0.24465876326889102</v>
+        <v>-0.03590555454326131</v>
+      </c>
+      <c r="F48" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49">
-        <v>376</v>
+        <v>264</v>
       </c>
       <c r="B49">
-        <v>320.15768707482994</v>
+        <v>217.60834467120182</v>
       </c>
       <c r="C49">
         <v>4</v>
       </c>
       <c r="D49">
-        <v>72.12462349910734</v>
+        <v>69.96807012672824</v>
       </c>
       <c r="E49">
-        <v>-0.020844377042223527</v>
+        <v>0.28819185858077745</v>
+      </c>
+      <c r="F49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50">
-        <v>380</v>
+        <v>268</v>
       </c>
       <c r="B50">
-        <v>323.48526077097506</v>
+        <v>221.03848072562357</v>
       </c>
       <c r="C50">
         <v>4</v>
       </c>
       <c r="D50">
-        <v>71.8694615901727</v>
+        <v>68.92285251004427</v>
       </c>
       <c r="E50">
-        <v>-0.06379047723365971</v>
+        <v>-0.26130440417099265</v>
+      </c>
+      <c r="F50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50">
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51">
-        <v>384</v>
+        <v>272</v>
       </c>
       <c r="B51">
-        <v>326.8246485260771</v>
+        <v>224.52063492063493</v>
       </c>
       <c r="C51">
         <v>4</v>
       </c>
       <c r="D51">
-        <v>71.55654413802887</v>
+        <v>70.06394725344566</v>
       </c>
       <c r="E51">
-        <v>-0.07822936303595895</v>
+        <v>0.28527368585034907</v>
+      </c>
+      <c r="F51" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51">
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52">
-        <v>388</v>
+        <v>276</v>
       </c>
       <c r="B52">
-        <v>330.17863945578233</v>
+        <v>227.94607709750568</v>
       </c>
       <c r="C52">
         <v>4</v>
       </c>
       <c r="D52">
-        <v>72.13642125925263</v>
+        <v>70.439782770738</v>
       </c>
       <c r="E52">
-        <v>0.14496928030593992</v>
+        <v>0.09395887932308611</v>
+      </c>
+      <c r="F52" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53">
-        <v>392</v>
+        <v>280</v>
       </c>
       <c r="B53">
-        <v>333.50566893424036</v>
+        <v>231.3532426303855</v>
       </c>
       <c r="C53">
         <v>4</v>
       </c>
       <c r="D53">
-        <v>71.89435930877136</v>
+        <v>71.07983049367705</v>
       </c>
       <c r="E53">
-        <v>-0.060515487620318</v>
+        <v>0.16001193073476117</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54">
-        <v>396</v>
+        <v>284</v>
       </c>
       <c r="B54">
-        <v>336.84390022675734</v>
+        <v>234.72972789115647</v>
       </c>
       <c r="C54">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D54">
-        <v>72.63005336085547</v>
+        <v>69.55150320354889</v>
       </c>
       <c r="E54">
-        <v>0.18392351302102838</v>
+        <v>-0.38208182253204015</v>
+      </c>
+      <c r="F54" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55">
-        <v>406</v>
+        <v>288</v>
       </c>
       <c r="B55">
-        <v>345.1049433106576</v>
+        <v>238.1804081632653</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D55">
-        <v>74.28306733482101</v>
+        <v>70.06348344730328</v>
       </c>
       <c r="E55">
-        <v>0.16530139739655425</v>
+        <v>0.12799506093859847</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56">
-        <v>412</v>
+        <v>292</v>
       </c>
       <c r="B56">
-        <v>349.95126984126983</v>
+        <v>241.60587301587302</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D56">
-        <v>74.70197553693731</v>
+        <v>70.6009485501591</v>
       </c>
       <c r="E56">
-        <v>0.06981803368604982</v>
+        <v>0.13436627571395476</v>
+      </c>
+      <c r="F56" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56">
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57">
-        <v>416</v>
+        <v>300</v>
       </c>
       <c r="B57">
-        <v>353.16403628117916</v>
+        <v>248.4046485260771</v>
       </c>
       <c r="C57">
         <v>4</v>
       </c>
       <c r="D57">
-        <v>74.45813137104669</v>
+        <v>69.46294850002286</v>
       </c>
       <c r="E57">
-        <v>-0.06096104147265535</v>
+        <v>-0.14225000626703022</v>
+      </c>
+      <c r="F57" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58">
-        <v>420</v>
+        <v>304</v>
       </c>
       <c r="B58">
-        <v>356.3873242630385</v>
+        <v>251.85972789115647</v>
       </c>
       <c r="C58">
         <v>4</v>
       </c>
       <c r="D58">
-        <v>74.7642425740821</v>
+        <v>69.73204814831918</v>
       </c>
       <c r="E58">
-        <v>0.07652780075885346</v>
+        <v>0.06727491207407965</v>
+      </c>
+      <c r="F58" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58">
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59">
-        <v>424</v>
+        <v>308</v>
       </c>
       <c r="B59">
-        <v>359.5974149659864</v>
+        <v>255.3014739229025</v>
       </c>
       <c r="C59">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D59">
-        <v>75.47385084929488</v>
+        <v>68.66841408662674</v>
       </c>
       <c r="E59">
-        <v>0.1774020688031932</v>
+        <v>-0.26590851542311</v>
+      </c>
+      <c r="F59" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59">
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60">
-        <v>432</v>
+        <v>312</v>
       </c>
       <c r="B60">
-        <v>365.9572335600907</v>
+        <v>258.7965306122449</v>
       </c>
       <c r="C60">
         <v>4</v>
       </c>
       <c r="D60">
-        <v>75.55089192025162</v>
+        <v>68.12652068126593</v>
       </c>
       <c r="E60">
-        <v>0.009630133869592328</v>
+        <v>-0.13547335134020244</v>
+      </c>
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60">
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61">
-        <v>436</v>
+        <v>316</v>
       </c>
       <c r="B61">
-        <v>369.13390022675736</v>
+        <v>262.319387755102</v>
       </c>
       <c r="C61">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D61">
-        <v>75.19573341416853</v>
+        <v>69.13580246913544</v>
       </c>
       <c r="E61">
-        <v>-0.08878962652077149</v>
+        <v>0.2523204469673779</v>
+      </c>
+      <c r="F61" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62">
-        <v>448</v>
+        <v>320</v>
       </c>
       <c r="B62">
-        <v>378.70891156462585</v>
+        <v>265.7908163265306</v>
       </c>
       <c r="C62">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D62">
-        <v>74.27316299534772</v>
+        <v>69.56681773217706</v>
       </c>
       <c r="E62">
-        <v>-0.07688086823506761</v>
+        <v>0.10775381576040388</v>
+      </c>
+      <c r="F62" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62">
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63">
-        <v>452</v>
+        <v>328</v>
       </c>
       <c r="B63">
-        <v>381.9402267573696</v>
+        <v>272.69065759637186</v>
       </c>
       <c r="C63">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D63">
-        <v>75.46416450389214</v>
+        <v>68.67754839839948</v>
       </c>
       <c r="E63">
-        <v>0.2977503771361043</v>
+        <v>-0.1111586667221971</v>
+      </c>
+      <c r="F63" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63">
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64">
-        <v>456</v>
+        <v>336</v>
       </c>
       <c r="B64">
-        <v>385.1205442176871</v>
+        <v>279.6798412698413</v>
       </c>
       <c r="C64">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D64">
-        <v>74.63823305407483</v>
+        <v>68.28959848245324</v>
       </c>
       <c r="E64">
-        <v>-0.206482862454326</v>
+        <v>-0.04849373949327962</v>
+      </c>
+      <c r="F64" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65">
-        <v>464</v>
+        <v>340</v>
       </c>
       <c r="B65">
-        <v>391.55156462585035</v>
+        <v>283.19428571428574</v>
       </c>
       <c r="C65">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D65">
-        <v>75.4647025689657</v>
+        <v>68.49820405785937</v>
       </c>
       <c r="E65">
-        <v>0.10330868936135928</v>
+        <v>0.052151393851531225</v>
+      </c>
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65">
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66">
-        <v>472</v>
+        <v>344</v>
       </c>
       <c r="B66">
-        <v>397.91215419501134</v>
+        <v>286.69802721088433</v>
       </c>
       <c r="C66">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D66">
-        <v>75.01328891881383</v>
+        <v>69.84801589134756</v>
       </c>
       <c r="E66">
-        <v>-0.056426706268984717</v>
+        <v>0.33745295837204736</v>
+      </c>
+      <c r="F66" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66">
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67">
-        <v>480</v>
+        <v>348</v>
       </c>
       <c r="B67">
-        <v>404.31102040816324</v>
+        <v>290.1340589569161</v>
       </c>
       <c r="C67">
         <v>4</v>
       </c>
       <c r="D67">
-        <v>74.29036695959753</v>
+        <v>70.26628692067077</v>
       </c>
       <c r="E67">
-        <v>-0.09036524490203668</v>
+        <v>0.10456775733080192</v>
+      </c>
+      <c r="F67" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68">
-        <v>484</v>
+        <v>352</v>
       </c>
       <c r="B68">
-        <v>407.5415873015873</v>
+        <v>293.54963718820864</v>
       </c>
       <c r="C68">
         <v>4</v>
       </c>
       <c r="D68">
-        <v>75.01063075832715</v>
+        <v>69.4944189100469</v>
       </c>
       <c r="E68">
-        <v>0.18006594968240464</v>
+        <v>-0.19296700265596556</v>
+      </c>
+      <c r="F68" t="s">
+        <v>8</v>
+      </c>
+      <c r="G68">
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69">
-        <v>488</v>
+        <v>356</v>
       </c>
       <c r="B69">
-        <v>410.7411337868481</v>
+        <v>297.0031519274376</v>
       </c>
       <c r="C69">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D69">
-        <v>72.14199376550678</v>
+        <v>70.13800301519191</v>
       </c>
       <c r="E69">
-        <v>-0.7171592482050926</v>
+        <v>0.16089602628625244</v>
+      </c>
+      <c r="F69" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69">
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70">
-        <v>494</v>
+        <v>364</v>
       </c>
       <c r="B70">
-        <v>415.7312925170068</v>
+        <v>303.8468027210884</v>
       </c>
       <c r="C70">
         <v>4</v>
       </c>
       <c r="D70">
-        <v>71.23818754543314</v>
+        <v>69.5437342304449</v>
       </c>
       <c r="E70">
-        <v>-0.15063437001227462</v>
+        <v>-0.07428359809337692</v>
+      </c>
+      <c r="F70" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70">
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71">
-        <v>498</v>
+        <v>368</v>
       </c>
       <c r="B71">
-        <v>419.1002721088435</v>
+        <v>307.29786848072564</v>
       </c>
       <c r="C71">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D71">
-        <v>71.26840797527404</v>
+        <v>69.86692015209114</v>
       </c>
       <c r="E71">
-        <v>0.007555107460227362</v>
+        <v>0.08079648041156062</v>
+      </c>
+      <c r="F71" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71">
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72">
-        <v>506</v>
+        <v>372</v>
       </c>
       <c r="B72">
-        <v>425.83537414965986</v>
+        <v>310.732970521542</v>
       </c>
       <c r="C72">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D72">
-        <v>72.34746469438235</v>
+        <v>70.08296859377221</v>
       </c>
       <c r="E72">
-        <v>0.13488208988853856</v>
+        <v>0.05401211042026688</v>
+      </c>
+      <c r="F72" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72">
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73">
-        <v>522</v>
+        <v>376</v>
       </c>
       <c r="B73">
-        <v>439.1046712018141</v>
+        <v>314.1574829931973</v>
       </c>
       <c r="C73">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D73">
-        <v>73.92197125256732</v>
+        <v>70.78178291981561</v>
       </c>
       <c r="E73">
-        <v>0.09840665988656028</v>
+        <v>0.17470358151085108</v>
+      </c>
+      <c r="F73" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73">
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74">
-        <v>530</v>
+        <v>380</v>
       </c>
       <c r="B74">
-        <v>445.59800453514737</v>
+        <v>317.5481859410431</v>
       </c>
       <c r="C74">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D74">
-        <v>72.91733646877232</v>
+        <v>70.01111287505958</v>
       </c>
       <c r="E74">
-        <v>-0.12557934797437476</v>
+        <v>-0.1926675111890077</v>
+      </c>
+      <c r="F74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74">
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75">
-        <v>542</v>
+        <v>384</v>
       </c>
       <c r="B75">
-        <v>455.4721995464853</v>
+        <v>320.9762131519274</v>
       </c>
       <c r="C75">
         <v>4</v>
       </c>
       <c r="D75">
-        <v>73.51327322988968</v>
+        <v>70.92360166453287</v>
       </c>
       <c r="E75">
-        <v>0.0496613967597798</v>
+        <v>0.22812219736832162</v>
+      </c>
+      <c r="F75" t="s">
+        <v>8</v>
+      </c>
+      <c r="G75">
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76">
-        <v>546</v>
+        <v>388</v>
       </c>
       <c r="B76">
-        <v>458.7369160997732</v>
+        <v>324.3601360544218</v>
       </c>
       <c r="C76">
         <v>4</v>
       </c>
       <c r="D76">
-        <v>74.08133268005795</v>
+        <v>72.50655943222452</v>
       </c>
       <c r="E76">
-        <v>0.1420148625420694</v>
+        <v>0.3957394419229132</v>
+      </c>
+      <c r="F76" t="s">
+        <v>8</v>
+      </c>
+      <c r="G76">
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77">
-        <v>550</v>
+        <v>392</v>
       </c>
       <c r="B77">
-        <v>461.9765986394558</v>
+        <v>327.6701814058957</v>
       </c>
       <c r="C77">
         <v>4</v>
       </c>
       <c r="D77">
-        <v>73.0354136189244</v>
+        <v>71.78513293543158</v>
       </c>
       <c r="E77">
-        <v>-0.26147976528339</v>
+        <v>-0.18035662419823595</v>
+      </c>
+      <c r="F77" t="s">
+        <v>8</v>
+      </c>
+      <c r="G77">
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78">
-        <v>554</v>
+        <v>396</v>
       </c>
       <c r="B78">
-        <v>465.26267573696146</v>
+        <v>331.01349206349204</v>
       </c>
       <c r="C78">
-        <v>0.03125</v>
+        <v>4</v>
       </c>
       <c r="D78">
-        <v>73.50612551052731</v>
+        <v>70.79740730583174</v>
       </c>
       <c r="E78">
-        <v>0.11767797290072934</v>
+        <v>-0.2469314073999591</v>
+      </c>
+      <c r="F78" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79">
-        <v>554.03125</v>
+        <v>400</v>
       </c>
       <c r="B79">
-        <v>465.2881838151927</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10"/>
+        <v>334.40344671201814</v>
+      </c>
+      <c r="C79">
+        <v>8</v>
+      </c>
+      <c r="D79">
+        <v>70.43673571250328</v>
+      </c>
+      <c r="E79">
+        <v>-0.09016789833211547</v>
+      </c>
+      <c r="F79" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80">
+        <v>408</v>
+      </c>
+      <c r="B80">
+        <v>341.21807256235826</v>
+      </c>
+      <c r="C80">
+        <v>8</v>
+      </c>
+      <c r="D80">
+        <v>70.2010386888373</v>
+      </c>
+      <c r="E80">
+        <v>-0.02946212795824721</v>
+      </c>
+      <c r="F80" t="s">
+        <v>9</v>
+      </c>
+      <c r="G80">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81">
+        <v>416</v>
+      </c>
+      <c r="B81">
+        <v>348.05557823129254</v>
+      </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+      <c r="D81">
+        <v>70.92882991556203</v>
+      </c>
+      <c r="E81">
+        <v>0.09097390334059163</v>
+      </c>
+      <c r="F81" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82">
+        <v>420</v>
+      </c>
+      <c r="B82">
+        <v>351.43925170068024</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <v>71.28760886110851</v>
+      </c>
+      <c r="E82">
+        <v>0.08969473638661896</v>
+      </c>
+      <c r="F82" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83">
+        <v>424</v>
+      </c>
+      <c r="B83">
+        <v>354.80589569161</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="D83">
+        <v>71.74085446448579</v>
+      </c>
+      <c r="E83">
+        <v>0.11331140084432079</v>
+      </c>
+      <c r="F83" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84">
+        <v>428</v>
+      </c>
+      <c r="B84">
+        <v>358.1512698412698</v>
+      </c>
+      <c r="C84">
+        <v>8</v>
+      </c>
+      <c r="D84">
+        <v>70.26372130848264</v>
+      </c>
+      <c r="E84">
+        <v>-0.3692832890007871</v>
+      </c>
+      <c r="F84" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85">
+        <v>436</v>
+      </c>
+      <c r="B85">
+        <v>364.9826757369614</v>
+      </c>
+      <c r="C85">
+        <v>4</v>
+      </c>
+      <c r="D85">
+        <v>70.7070707070704</v>
+      </c>
+      <c r="E85">
+        <v>0.055418674823469516</v>
+      </c>
+      <c r="F85" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86">
+        <v>440</v>
+      </c>
+      <c r="B86">
+        <v>368.37696145124715</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="D86">
+        <v>72.22108495394099</v>
+      </c>
+      <c r="E86">
+        <v>0.3785035617176469</v>
+      </c>
+      <c r="F86" t="s">
+        <v>9</v>
+      </c>
+      <c r="G86">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87">
+        <v>444</v>
+      </c>
+      <c r="B87">
+        <v>371.7000907029478</v>
+      </c>
+      <c r="C87">
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <v>70.39059330544391</v>
+      </c>
+      <c r="E87">
+        <v>-0.4576229121242683</v>
+      </c>
+      <c r="F87" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88">
+        <v>448</v>
+      </c>
+      <c r="B88">
+        <v>375.10963718820864</v>
+      </c>
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="D88">
+        <v>71.43242805464091</v>
+      </c>
+      <c r="E88">
+        <v>0.2604586872992485</v>
+      </c>
+      <c r="F88" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89">
+        <v>452</v>
+      </c>
+      <c r="B89">
+        <v>378.46945578231293</v>
+      </c>
+      <c r="C89">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>68.00439484184348</v>
+      </c>
+      <c r="E89">
+        <v>-0.8570083031993576</v>
+      </c>
+      <c r="F89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90">
+        <v>456</v>
+      </c>
+      <c r="B90">
+        <v>381.9986394557823</v>
+      </c>
+      <c r="C90">
+        <v>12</v>
+      </c>
+      <c r="D90">
+        <v>70.09395309409459</v>
+      </c>
+      <c r="E90">
+        <v>0.5223895630627773</v>
+      </c>
+      <c r="F90" t="s">
+        <v>7</v>
+      </c>
+      <c r="G90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91">
+        <v>468</v>
+      </c>
+      <c r="B91">
+        <v>392.270566893424</v>
+      </c>
+      <c r="C91">
+        <v>4</v>
+      </c>
+      <c r="D91">
+        <v>69.18913265172702</v>
+      </c>
+      <c r="E91">
+        <v>-0.07540170353063047</v>
+      </c>
+      <c r="F91" t="s">
+        <v>10</v>
+      </c>
+      <c r="G91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92">
+        <v>472</v>
+      </c>
+      <c r="B92">
+        <v>395.73931972789114</v>
+      </c>
+      <c r="C92">
+        <v>4</v>
+      </c>
+      <c r="D92">
+        <v>69.63157894736818</v>
+      </c>
+      <c r="E92">
+        <v>0.11061157391029042</v>
+      </c>
+      <c r="F92" t="s">
+        <v>10</v>
+      </c>
+      <c r="G92">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93">
+        <v>476</v>
+      </c>
+      <c r="B93">
+        <v>399.18603174603174</v>
+      </c>
+      <c r="C93">
+        <v>4</v>
+      </c>
+      <c r="D93">
+        <v>69.27608325697132</v>
+      </c>
+      <c r="E93">
+        <v>-0.08887392259921612</v>
+      </c>
+      <c r="F93" t="s">
+        <v>10</v>
+      </c>
+      <c r="G93">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94">
+        <v>480</v>
+      </c>
+      <c r="B94">
+        <v>402.65043083900224</v>
+      </c>
+      <c r="C94">
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <v>70.385444098635</v>
+      </c>
+      <c r="E94">
+        <v>0.2773402104159217</v>
+      </c>
+      <c r="F94" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95">
+        <v>484</v>
+      </c>
+      <c r="B95">
+        <v>406.0602267573696</v>
+      </c>
+      <c r="C95">
+        <v>4</v>
+      </c>
+      <c r="D95">
+        <v>71.28040731661245</v>
+      </c>
+      <c r="E95">
+        <v>0.22374080449436207</v>
+      </c>
+      <c r="F95" t="s">
+        <v>10</v>
+      </c>
+      <c r="G95">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96">
+        <v>488</v>
+      </c>
+      <c r="B96">
+        <v>409.42721088435377</v>
+      </c>
+      <c r="C96">
+        <v>4</v>
+      </c>
+      <c r="D96">
+        <v>72.22502763712883</v>
+      </c>
+      <c r="E96">
+        <v>0.23615508012909459</v>
+      </c>
+      <c r="F96" t="s">
+        <v>10</v>
+      </c>
+      <c r="G96">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97">
+        <v>492</v>
+      </c>
+      <c r="B97">
+        <v>412.7501587301587</v>
+      </c>
+      <c r="C97">
+        <v>4</v>
+      </c>
+      <c r="D97">
+        <v>68.84350201639103</v>
+      </c>
+      <c r="E97">
+        <v>-0.845381405184451</v>
+      </c>
+      <c r="F97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98">
+        <v>496</v>
+      </c>
+      <c r="B98">
+        <v>416.23632653061225</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98">
+        <v>68.61232480649251</v>
+      </c>
+      <c r="E98">
+        <v>-0.05779430247462969</v>
+      </c>
+      <c r="F98" t="s">
+        <v>6</v>
+      </c>
+      <c r="G98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99">
+        <v>500</v>
+      </c>
+      <c r="B99">
+        <v>419.7342403628118</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+      <c r="D99">
+        <v>69.93709361949597</v>
+      </c>
+      <c r="E99">
+        <v>0.33119220325086474</v>
+      </c>
+      <c r="F99" t="s">
+        <v>6</v>
+      </c>
+      <c r="G99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100">
+        <v>504</v>
+      </c>
+      <c r="B100">
+        <v>423.16589569161</v>
+      </c>
+      <c r="C100">
+        <v>8</v>
+      </c>
+      <c r="D100">
+        <v>68.51461049469825</v>
+      </c>
+      <c r="E100">
+        <v>-0.3556207811994305</v>
+      </c>
+      <c r="F100" t="s">
+        <v>6</v>
+      </c>
+      <c r="G100">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101">
+        <v>512</v>
+      </c>
+      <c r="B101">
+        <v>430.1717006802721</v>
+      </c>
+      <c r="C101">
+        <v>4</v>
+      </c>
+      <c r="D101">
+        <v>70.38076365522456</v>
+      </c>
+      <c r="E101">
+        <v>0.23326914506578866</v>
+      </c>
+      <c r="F101" t="s">
+        <v>6</v>
+      </c>
+      <c r="G101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102">
+        <v>516</v>
+      </c>
+      <c r="B102">
+        <v>433.5817233560091</v>
+      </c>
+      <c r="C102">
+        <v>4</v>
+      </c>
+      <c r="D102">
+        <v>69.32599724896865</v>
+      </c>
+      <c r="E102">
+        <v>-0.263691601563977</v>
+      </c>
+      <c r="F102" t="s">
+        <v>6</v>
+      </c>
+      <c r="G102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103">
+        <v>520</v>
+      </c>
+      <c r="B103">
+        <v>437.04362811791384</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103">
+        <v>69.55835962145112</v>
+      </c>
+      <c r="E103">
+        <v>0.058090593120617484</v>
+      </c>
+      <c r="F103" t="s">
+        <v>6</v>
+      </c>
+      <c r="G103">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104">
+        <v>524</v>
+      </c>
+      <c r="B104">
+        <v>440.49396825396826</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104">
+        <v>69.22080809930601</v>
+      </c>
+      <c r="E104">
+        <v>-0.08438788053627633</v>
+      </c>
+      <c r="F104" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105">
+        <v>528</v>
+      </c>
+      <c r="B105">
+        <v>443.96113378684805</v>
+      </c>
+      <c r="C105">
+        <v>8</v>
+      </c>
+      <c r="D105">
+        <v>69.3946327998478</v>
+      </c>
+      <c r="E105">
+        <v>0.04345617513544653</v>
+      </c>
+      <c r="F105" t="s">
+        <v>11</v>
+      </c>
+      <c r="G105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106">
+        <v>536</v>
+      </c>
+      <c r="B106">
+        <v>450.8780952380952</v>
+      </c>
+      <c r="C106">
+        <v>0.03125</v>
+      </c>
+      <c r="D106">
+        <v>69.1511603596067</v>
+      </c>
+      <c r="E106">
+        <v>-0.03043405503013652</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107">
+        <v>536.03125</v>
+      </c>
+      <c r="B107">
+        <v>450.9052097505669</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>